<commit_message>
updated basic file and added an excel sheet for tracking python topics list
</commit_message>
<xml_diff>
--- a/Python_Topics.xlsx
+++ b/Python_Topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnc11\git_projects\Python_Arsenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947818A0-4B62-4F74-9F6F-757FD2D1279C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7E996-7A0E-492A-80C3-715667D713EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Python</t>
   </si>
@@ -97,13 +97,106 @@
   </si>
   <si>
     <t>Using Python generators to create iterators</t>
+  </si>
+  <si>
+    <t>Python Basics</t>
+  </si>
+  <si>
+    <t>Difference between Method and Function in Python</t>
+  </si>
+  <si>
+    <t>What can Python do?</t>
+  </si>
+  <si>
+    <t>Why Python?</t>
+  </si>
+  <si>
+    <t>Python Syntax compared to other programming languages</t>
+  </si>
+  <si>
+    <t>Structuring with Indentation</t>
+  </si>
+  <si>
+    <t>Operators</t>
+  </si>
+  <si>
+    <t>Precedence of Logical Operators</t>
+  </si>
+  <si>
+    <t>Assignment Expressions</t>
+  </si>
+  <si>
+    <t>Data Types and Variables</t>
+  </si>
+  <si>
+    <t>Valid Variable Names</t>
+  </si>
+  <si>
+    <t>Python Keywords</t>
+  </si>
+  <si>
+    <t>Naming Conventions</t>
+  </si>
+  <si>
+    <t>Changing Data Types and Storage Locations</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Integer Division</t>
+  </si>
+  <si>
+    <t>Floor Division</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Continuation of statements</t>
+  </si>
+  <si>
+    <t>Python Boolean</t>
+  </si>
+  <si>
+    <t>Python Constants</t>
+  </si>
+  <si>
+    <t>Python Type Conversion</t>
+  </si>
+  <si>
+    <t>Python Integers</t>
+  </si>
+  <si>
+    <t>Python Floor Division</t>
+  </si>
+  <si>
+    <t>Python Modulo</t>
+  </si>
+  <si>
+    <t>Python and Operator</t>
+  </si>
+  <si>
+    <t>Python or Operator</t>
+  </si>
+  <si>
+    <t>Python float</t>
+  </si>
+  <si>
+    <t>Python Rounding</t>
+  </si>
+  <si>
+    <t>Python Decimal</t>
+  </si>
+  <si>
+    <t>Print function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,15 +206,21 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -148,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,22 +270,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,79 +609,81 @@
     <col min="21" max="21" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="K1" s="2" t="s">
+    <row r="1" spans="1:21" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="72" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:21" ht="105" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -575,8 +707,10 @@
       <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -594,14 +728,16 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -623,8 +759,10 @@
       <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -645,9 +783,11 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -668,9 +808,11 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+    <row r="8" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -692,8 +834,10 @@
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -714,9 +858,11 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+    <row r="10" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -737,9 +883,11 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+    <row r="11" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -760,9 +908,11 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+    <row r="12" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -783,6 +933,111 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
+    <row r="13" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
made few changes in Python basics and control flow file w.r.t indexing
</commit_message>
<xml_diff>
--- a/Python_Topics.xlsx
+++ b/Python_Topics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnc11\git_projects\Python_Arsenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7E996-7A0E-492A-80C3-715667D713EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFF9A4E-5C0F-496F-BE0F-CADAA1A2C257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Python</t>
   </si>
@@ -190,13 +190,91 @@
   </si>
   <si>
     <t>Print function</t>
+  </si>
+  <si>
+    <t>Data pretty printer</t>
+  </si>
+  <si>
+    <t>Basics</t>
+  </si>
+  <si>
+    <t>Python if statement</t>
+  </si>
+  <si>
+    <t>Python if…else statement</t>
+  </si>
+  <si>
+    <t>Python if…elif…else statement</t>
+  </si>
+  <si>
+    <t>Python Ternary Operator</t>
+  </si>
+  <si>
+    <t>Python for Loop with Range</t>
+  </si>
+  <si>
+    <t>Python while</t>
+  </si>
+  <si>
+    <t>Python break</t>
+  </si>
+  <si>
+    <t>Python continue</t>
+  </si>
+  <si>
+    <t>Python pass</t>
+  </si>
+  <si>
+    <t>Python for else</t>
+  </si>
+  <si>
+    <t>Python while else</t>
+  </si>
+  <si>
+    <t>Python do…while Loop Statement Emulation</t>
+  </si>
+  <si>
+    <t>declaration of lists</t>
+  </si>
+  <si>
+    <t>Accessing,Slicing and indexing</t>
+  </si>
+  <si>
+    <t>Basic List Operations</t>
+  </si>
+  <si>
+    <t>Built-in List Functions &amp; Methods</t>
+  </si>
+  <si>
+    <t>Main methods used in lists</t>
+  </si>
+  <si>
+    <t>List comprehension</t>
+  </si>
+  <si>
+    <t>Lambda, The map(), the Filter and reduce() functions</t>
+  </si>
+  <si>
+    <t>Updating Lists</t>
+  </si>
+  <si>
+    <t>Delete List Elements.</t>
+  </si>
+  <si>
+    <t>How to Use a For Loop to Iterate over a List?</t>
+  </si>
+  <si>
+    <t>Python Iterables</t>
+  </si>
+  <si>
+    <t>Tricks and questions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +303,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -298,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -316,6 +401,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -598,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,12 +771,16 @@
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -710,12 +802,16 @@
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -737,12 +833,16 @@
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -758,16 +858,20 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -787,12 +891,16 @@
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -812,12 +920,16 @@
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -837,12 +949,16 @@
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -858,16 +974,20 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -887,12 +1007,16 @@
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -912,12 +1036,16 @@
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -937,15 +1065,33 @@
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>36</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
@@ -1036,6 +1182,11 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formatted list python file but not completed yet
</commit_message>
<xml_diff>
--- a/Python_Topics.xlsx
+++ b/Python_Topics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnc11\git_projects\Python_Arsenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFF9A4E-5C0F-496F-BE0F-CADAA1A2C257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41F6818-0730-4CBB-B758-04244D31F617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,13 +303,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -383,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -401,9 +394,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -689,7 +679,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +761,7 @@
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="3"/>
@@ -802,7 +792,7 @@
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C4" s="3"/>
@@ -833,7 +823,7 @@
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="3"/>
@@ -862,7 +852,7 @@
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="3"/>
@@ -891,7 +881,7 @@
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C7" s="3"/>
@@ -920,7 +910,7 @@
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="3"/>
@@ -949,7 +939,7 @@
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C9" s="3"/>
@@ -974,11 +964,11 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="3"/>
@@ -1007,7 +997,7 @@
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="3"/>
@@ -1036,7 +1026,7 @@
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C12" s="3"/>
@@ -1061,11 +1051,11 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4" t="s">
         <v>78</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -1076,7 +1066,7 @@
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1087,7 +1077,7 @@
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>80</v>
       </c>
       <c r="G15" s="4" t="s">

</xml_diff>